<commit_message>
Rodou na Produção Jayme
</commit_message>
<xml_diff>
--- a/Planilha de Configuração.xlsx
+++ b/Planilha de Configuração.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\LA VITA\TI\BotCity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guido\Desktop\GitHub Repositories\PrimeiroBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA6EE56-020A-4EDA-81AE-B002B382A07C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575F1375-AFC5-41D6-B4F8-5CA26F2E87DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9276" yWindow="2544" windowWidth="34560" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15420" yWindow="-5835" windowWidth="12150" windowHeight="20745" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
@@ -165,9 +165,6 @@
     <t>ENZYFOR</t>
   </si>
   <si>
-    <t>GGT</t>
-  </si>
-  <si>
     <t>JEJ</t>
   </si>
   <si>
@@ -967,6 +964,9 @@
   </si>
   <si>
     <t>PREGOMIN PLUS 1.0 KCAL 0 A 3 A</t>
+  </si>
+  <si>
+    <t>GTT</t>
   </si>
 </sst>
 </file>
@@ -1087,9 +1087,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1127,7 +1127,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1233,7 +1233,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1375,7 +1375,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1385,18 +1385,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B246"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1404,215 +1404,215 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B13" s="7">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="7">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" s="7">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B16" s="7">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B17" s="7">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="B18" s="7">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>108</v>
       </c>
       <c r="B19" s="7">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" s="7">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B21" s="7">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="7">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B23" s="7">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B24" s="7">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B25" s="7">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B26" s="7">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B27" s="7">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>25</v>
       </c>
@@ -1620,191 +1620,191 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B29" s="7">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B30" s="7">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B31" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B32" s="7">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B33" s="7">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B34" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B35" s="7">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B36" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B37" s="7">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B38" s="7">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B39" s="7">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B40" s="7">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B41" s="7">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B42" s="7">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B43" s="7">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B44" s="7">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B45" s="7">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B46" s="7">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B47" s="7">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B48" s="7">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B49" s="7">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B50" s="7">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B51" s="7">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>26</v>
       </c>
@@ -1812,175 +1812,175 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B53" s="7">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B54" s="7">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B55" s="7">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B56" s="7">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B57" s="7">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B58" s="7">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B59" s="7">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B60" s="7">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B61" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B62" s="7">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B63" s="7">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B64" s="7">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B65" s="7">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B66" s="7">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B67" s="7">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B68" s="7">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B69" s="7">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B70" s="7">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B71" s="7">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B72" s="7">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B73" s="7">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>27</v>
       </c>
@@ -1988,199 +1988,199 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B75" s="7">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B76" s="7">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B77" s="7">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B78" s="7">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B79" s="7">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B80" s="7">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B81" s="7">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B82" s="7">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B83" s="7">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B84" s="7">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B85" s="7">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B86" s="7">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B87" s="7">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B88" s="7">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B89" s="7">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B90" s="7">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B91" s="7">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B92" s="7">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B93" s="7">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B94" s="7">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B95" s="7">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B96" s="7">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B97" s="7">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B98" s="7">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>28</v>
       </c>
@@ -2188,23 +2188,23 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B100" s="7">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B101" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>29</v>
       </c>
@@ -2212,15 +2212,15 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B103" s="7">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>30</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>31</v>
       </c>
@@ -2236,23 +2236,23 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B106" s="7">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B107" s="7">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>32</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>33</v>
       </c>
@@ -2268,15 +2268,15 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B110" s="7">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>34</v>
       </c>
@@ -2284,103 +2284,103 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B112" s="7">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B113" s="7">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B114" s="7">
         <v>999</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B115" s="7">
         <v>1000</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B116" s="7">
         <v>1001</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B117" s="7">
         <v>1002</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B118" s="7">
         <v>1003</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B119" s="7">
         <v>1004</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B120" s="7">
         <v>1005</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B121" s="7">
         <v>1006</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B122" s="7">
         <v>1007</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B123" s="7">
         <v>1008</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>35</v>
       </c>
@@ -2388,23 +2388,23 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B125" s="7">
         <v>1010</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B126" s="7">
         <v>1011</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>36</v>
       </c>
@@ -2412,87 +2412,87 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B128" s="7">
         <v>1013</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B129" s="7">
         <v>1014</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B130" s="7">
         <v>1015</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B131" s="7">
         <v>1016</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B132" s="7">
         <v>1017</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B133" s="7">
         <v>1018</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B134" s="7">
         <v>1019</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B135" s="7">
         <v>1020</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B136" s="7">
         <v>1021</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B137" s="7">
         <v>1022</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>37</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>38</v>
       </c>
@@ -2508,47 +2508,47 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B140" s="7">
         <v>1025</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B141" s="7">
         <v>1026</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B142" s="7">
         <v>1027</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B143" s="7">
         <v>1028</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B144" s="7">
         <v>1029</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
         <v>39</v>
       </c>
@@ -2556,63 +2556,63 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B146" s="7">
         <v>1031</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B147" s="7">
         <v>1032</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B148" s="7">
         <v>1033</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B149" s="7">
         <v>1035</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B150" s="7">
         <v>1036</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B151" s="7">
         <v>1037</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B152" s="7">
         <v>1038</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
         <v>40</v>
       </c>
@@ -2620,327 +2620,327 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B154" s="7">
         <v>1040</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B155" s="7">
         <v>1041</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B156" s="7">
         <v>1042</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B157" s="7">
         <v>1043</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B158" s="7">
         <v>1044</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B159" s="7">
         <v>1045</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B160" s="7">
         <v>1046</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B161" s="7">
         <v>1047</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B162" s="7">
         <v>1048</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B163" s="7">
         <v>1049</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B164" s="7">
         <v>1050</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B165" s="7">
         <v>1051</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B166" s="7">
         <v>1052</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B167" s="7">
         <v>1053</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B168" s="7">
         <v>1054</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B169" s="7">
         <v>1055</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B170" s="7">
         <v>1056</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B171" s="7">
         <v>1057</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B172" s="7">
         <v>1058</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B173" s="7">
         <v>1059</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B174" s="7">
         <v>1060</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B175" s="7">
         <v>1061</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B176" s="7">
         <v>1063</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B177" s="7">
         <v>1064</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B178" s="7">
         <v>1065</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B179" s="7">
         <v>1066</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B180" s="7">
         <v>1067</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B181" s="7">
         <v>1068</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B182" s="7">
         <v>1069</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B183" s="7">
         <v>1070</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B184" s="7">
         <v>1071</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B185" s="7">
         <v>1072</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B186" s="7">
         <v>1073</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B187" s="7">
         <v>1074</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B188" s="7">
         <v>1075</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B189" s="7">
         <v>1076</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B190" s="7">
         <v>1077</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B191" s="7">
         <v>1078</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B192" s="7">
         <v>1079</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B193" s="7">
         <v>1080</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="7" t="s">
         <v>41</v>
       </c>
@@ -2948,71 +2948,71 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B195" s="7">
         <v>1082</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B196" s="7">
         <v>1083</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B197" s="7">
         <v>1084</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B198" s="7">
         <v>1085</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B199" s="7">
         <v>1086</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B200" s="7">
         <v>1087</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B201" s="7">
         <v>1088</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B202" s="7">
         <v>1089</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="7" t="s">
         <v>42</v>
       </c>
@@ -3020,23 +3020,23 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B204" s="7">
         <v>1091</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B205" s="7">
         <v>1092</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="7" t="s">
         <v>43</v>
       </c>
@@ -3044,143 +3044,143 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B207" s="7">
         <v>1094</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B208" s="7">
         <v>1095</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B209" s="7">
         <v>1096</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B210" s="7">
         <v>1097</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B211" s="7">
         <v>1098</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B212" s="7">
         <v>1099</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B213" s="7">
         <v>1100</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B214" s="7">
         <v>1101</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B215" s="7">
         <v>1102</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B216" s="7">
         <v>1103</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B217" s="7">
         <v>1104</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B218" s="7">
         <v>1105</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B219" s="7">
         <v>1106</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B220" s="7">
         <v>1107</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B221" s="7">
         <v>1108</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B222" s="7">
         <v>1109</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B223" s="7">
         <v>1110</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="7" t="s">
         <v>44</v>
       </c>
@@ -3188,177 +3188,177 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B225" s="7">
         <v>1112</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B226" s="7">
         <v>1113</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B227" s="7">
         <v>1114</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B228" s="7">
         <v>1115</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B229" s="7">
         <v>1116</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B230" s="7">
         <v>1117</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B231" s="7">
         <v>1118</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B232" s="7">
         <v>1119</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B233" s="7">
         <v>1120</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B234" s="7">
         <v>1121</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B235" s="7">
         <v>1122</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B236" s="7">
         <v>1123</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B237" s="7">
         <v>1124</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B238" s="7">
         <v>1125</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B239" s="7">
         <v>1126</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B240" s="7">
         <v>1127</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B241" s="7">
         <v>1128</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B242" s="7">
         <v>1129</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B243" s="7">
         <v>1131</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B244" s="7">
         <v>1132</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B245" s="7">
         <v>1133</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B246" s="7">
         <v>1134</v>
@@ -3374,17 +3374,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3392,23 +3392,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -3441,7 +3441,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B7">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3458,18 +3458,18 @@
       <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -3484,12 +3484,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>4</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
@@ -3498,15 +3498,15 @@
         <v>50</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>4</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="9">
         <v>51</v>
@@ -3515,15 +3515,15 @@
         <v>100</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="9">
         <v>101</v>
@@ -3532,15 +3532,15 @@
         <v>150</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="9">
         <v>151</v>
@@ -3549,10 +3549,10 @@
         <v>200</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>4</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>4</v>
       </c>
@@ -3603,12 +3603,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>4</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" s="9">
         <v>1</v>
@@ -3617,15 +3617,15 @@
         <v>100</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>4</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" s="9">
         <v>101</v>
@@ -3634,15 +3634,15 @@
         <v>240</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>4</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
@@ -3651,15 +3651,15 @@
         <v>100</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>4</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" s="9">
         <v>101</v>
@@ -3668,15 +3668,15 @@
         <v>240</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>4</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="9">
         <v>1</v>
@@ -3685,15 +3685,15 @@
         <v>100</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>4</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="9">
         <v>101</v>
@@ -3702,10 +3702,10 @@
         <v>240</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>4</v>
       </c>
@@ -3719,10 +3719,10 @@
         <v>20</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>4</v>
       </c>
@@ -3736,10 +3736,10 @@
         <v>40</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>4</v>
       </c>
@@ -3753,10 +3753,10 @@
         <v>60</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>4</v>
       </c>
@@ -3770,10 +3770,10 @@
         <v>80</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>4</v>
       </c>
@@ -3787,10 +3787,10 @@
         <v>100</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>4</v>
       </c>
@@ -3804,10 +3804,10 @@
         <v>120</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>4</v>
       </c>
@@ -3821,15 +3821,15 @@
         <v>160</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
@@ -3838,15 +3838,15 @@
         <v>50</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>25</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" s="2">
         <v>51</v>
@@ -3855,15 +3855,15 @@
         <v>100</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>25</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C24" s="2">
         <v>101</v>
@@ -3872,15 +3872,15 @@
         <v>150</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C25" s="2">
         <v>151</v>
@@ -3889,10 +3889,10 @@
         <v>200</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>25</v>
       </c>
@@ -3943,12 +3943,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29" s="2">
         <v>1</v>
@@ -3957,15 +3957,15 @@
         <v>100</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>25</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C30" s="2">
         <v>101</v>
@@ -3974,15 +3974,15 @@
         <v>240</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>25</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" s="2">
         <v>1</v>
@@ -3991,15 +3991,15 @@
         <v>100</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>25</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" s="2">
         <v>101</v>
@@ -4008,15 +4008,15 @@
         <v>240</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>25</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
@@ -4025,15 +4025,15 @@
         <v>100</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>25</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" s="2">
         <v>101</v>
@@ -4042,10 +4042,10 @@
         <v>240</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>25</v>
       </c>
@@ -4059,10 +4059,10 @@
         <v>10</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>25</v>
       </c>
@@ -4076,10 +4076,10 @@
         <v>20</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>25</v>
       </c>
@@ -4093,10 +4093,10 @@
         <v>30</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>25</v>
       </c>
@@ -4110,10 +4110,10 @@
         <v>40</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>25</v>
       </c>
@@ -4127,10 +4127,10 @@
         <v>60</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>25</v>
       </c>
@@ -4144,10 +4144,10 @@
         <v>70</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>25</v>
       </c>
@@ -4161,10 +4161,10 @@
         <v>120</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>25</v>
       </c>
@@ -4178,10 +4178,10 @@
         <v>130</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>25</v>
       </c>
@@ -4195,10 +4195,10 @@
         <v>180</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>28</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>28</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>28</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>28</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>28</v>
       </c>
@@ -4280,10 +4280,10 @@
         <v>50</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>28</v>
       </c>
@@ -4297,10 +4297,10 @@
         <v>60</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>28</v>
       </c>
@@ -4314,10 +4314,10 @@
         <v>70</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>28</v>
       </c>
@@ -4331,10 +4331,10 @@
         <v>80</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>28</v>
       </c>
@@ -4348,10 +4348,10 @@
         <v>90</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>28</v>
       </c>
@@ -4365,10 +4365,10 @@
         <v>100</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>28</v>
       </c>
@@ -4382,15 +4382,15 @@
         <v>110</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>28</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C55" s="9">
         <v>1</v>
@@ -4399,15 +4399,15 @@
         <v>50</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>28</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C56" s="9">
         <v>51</v>
@@ -4416,15 +4416,15 @@
         <v>100</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>28</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C57" s="9">
         <v>101</v>
@@ -4433,15 +4433,15 @@
         <v>150</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>28</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C58" s="9">
         <v>151</v>
@@ -4450,15 +4450,15 @@
         <v>200</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>28</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C59" s="9">
         <v>1</v>
@@ -4467,15 +4467,15 @@
         <v>100</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>28</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C60" s="9">
         <v>101</v>
@@ -4484,15 +4484,15 @@
         <v>240</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>28</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C61" s="9">
         <v>1</v>
@@ -4501,15 +4501,15 @@
         <v>100</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>28</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C62" s="9">
         <v>101</v>
@@ -4518,15 +4518,15 @@
         <v>240</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>28</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C63" s="9">
         <v>1</v>
@@ -4535,15 +4535,15 @@
         <v>100</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>28</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C64" s="9">
         <v>101</v>
@@ -4552,10 +4552,10 @@
         <v>240</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>28</v>
       </c>
@@ -4569,10 +4569,10 @@
         <v>100</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <v>28</v>
       </c>
@@ -4586,10 +4586,10 @@
         <v>300</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>28</v>
       </c>
@@ -4603,12 +4603,12 @@
         <v>500</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>17</v>
@@ -4623,9 +4623,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>17</v>
@@ -4640,9 +4640,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>17</v>
@@ -4657,9 +4657,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>17</v>
@@ -4674,9 +4674,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>17</v>
@@ -4688,12 +4688,12 @@
         <v>50</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>17</v>
@@ -4705,12 +4705,12 @@
         <v>60</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>17</v>
@@ -4722,12 +4722,12 @@
         <v>70</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>17</v>
@@ -4739,12 +4739,12 @@
         <v>80</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>17</v>
@@ -4756,12 +4756,12 @@
         <v>90</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>17</v>
@@ -4773,12 +4773,12 @@
         <v>100</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>17</v>
@@ -4790,15 +4790,15 @@
         <v>110</v>
       </c>
       <c r="E78" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="C79" s="2">
         <v>1</v>
@@ -4807,15 +4807,15 @@
         <v>50</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C80" s="2">
         <v>51</v>
@@ -4824,15 +4824,15 @@
         <v>100</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C81" s="2">
         <v>101</v>
@@ -4841,15 +4841,15 @@
         <v>150</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C82" s="2">
         <v>151</v>
@@ -4858,12 +4858,12 @@
         <v>200</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>18</v>
@@ -4878,9 +4878,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>18</v>
@@ -4895,9 +4895,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>18</v>
@@ -4912,12 +4912,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C86" s="2">
         <v>1</v>
@@ -4926,15 +4926,15 @@
         <v>100</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C87" s="2">
         <v>101</v>
@@ -4943,15 +4943,15 @@
         <v>240</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C88" s="2">
         <v>1</v>
@@ -4960,15 +4960,15 @@
         <v>100</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C89" s="2">
         <v>101</v>
@@ -4977,15 +4977,15 @@
         <v>240</v>
       </c>
       <c r="E89" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="C90" s="2">
         <v>1</v>
@@ -4994,15 +4994,15 @@
         <v>100</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C91" s="2">
         <v>101</v>
@@ -5011,7 +5011,7 @@
         <v>240</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -5029,18 +5029,18 @@
       <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -5055,9 +5055,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>17</v>
@@ -5072,9 +5072,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>17</v>
@@ -5089,9 +5089,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>17</v>
@@ -5106,9 +5106,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
@@ -5123,9 +5123,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>17</v>
@@ -5137,12 +5137,12 @@
         <v>50</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>17</v>
@@ -5154,12 +5154,12 @@
         <v>60</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
@@ -5171,12 +5171,12 @@
         <v>70</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
@@ -5188,12 +5188,12 @@
         <v>80</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>17</v>
@@ -5205,12 +5205,12 @@
         <v>90</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>17</v>
@@ -5222,12 +5222,12 @@
         <v>100</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>17</v>
@@ -5239,15 +5239,15 @@
         <v>110</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -5256,15 +5256,15 @@
         <v>50</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="2">
         <v>51</v>
@@ -5273,15 +5273,15 @@
         <v>100</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="2">
         <v>101</v>
@@ -5290,15 +5290,15 @@
         <v>150</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2">
         <v>151</v>
@@ -5307,12 +5307,12 @@
         <v>200</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>18</v>
@@ -5327,9 +5327,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
@@ -5344,9 +5344,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>18</v>
@@ -5361,12 +5361,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
@@ -5375,15 +5375,15 @@
         <v>100</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="2">
         <v>101</v>
@@ -5392,15 +5392,15 @@
         <v>240</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="2">
         <v>1</v>
@@ -5409,15 +5409,15 @@
         <v>100</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="2">
         <v>101</v>
@@ -5426,15 +5426,15 @@
         <v>240</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="C24" s="2">
         <v>1</v>
@@ -5443,15 +5443,15 @@
         <v>100</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" s="2">
         <v>101</v>
@@ -5460,10 +5460,10 @@
         <v>240</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>28</v>
       </c>
@@ -5477,10 +5477,10 @@
         <v>100</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>28</v>
       </c>
@@ -5494,10 +5494,10 @@
         <v>300</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>28</v>
       </c>
@@ -5511,10 +5511,10 @@
         <v>500</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>25</v>
       </c>
@@ -5528,10 +5528,10 @@
         <v>10</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>25</v>
       </c>
@@ -5545,10 +5545,10 @@
         <v>20</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>25</v>
       </c>
@@ -5562,10 +5562,10 @@
         <v>30</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>25</v>
       </c>
@@ -5579,10 +5579,10 @@
         <v>40</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>25</v>
       </c>
@@ -5596,10 +5596,10 @@
         <v>60</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>25</v>
       </c>
@@ -5613,10 +5613,10 @@
         <v>70</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>25</v>
       </c>
@@ -5630,10 +5630,10 @@
         <v>120</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>25</v>
       </c>
@@ -5647,10 +5647,10 @@
         <v>130</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>25</v>
       </c>
@@ -5664,10 +5664,10 @@
         <v>180</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>4</v>
       </c>
@@ -5681,10 +5681,10 @@
         <v>20</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>4</v>
       </c>
@@ -5698,10 +5698,10 @@
         <v>40</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>4</v>
       </c>
@@ -5715,10 +5715,10 @@
         <v>60</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>4</v>
       </c>
@@ -5732,10 +5732,10 @@
         <v>80</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>4</v>
       </c>
@@ -5749,10 +5749,10 @@
         <v>100</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>4</v>
       </c>
@@ -5766,10 +5766,10 @@
         <v>120</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>4</v>
       </c>
@@ -5783,7 +5783,7 @@
         <v>160</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculos Seringas + Sleeps
</commit_message>
<xml_diff>
--- a/Planilha de Configuração.xlsx
+++ b/Planilha de Configuração.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\LA VITA\TI\OptiVita\Bots\01-Lançamento Prescrição\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Guido\Desktop\Github Repositories\PrimeiroBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1483A56D-F7B1-490C-A013-5490F815D38D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D41A222-91DA-47B2-9897-E3190675C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3250" yWindow="1520" windowWidth="31020" windowHeight="18110" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11295" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
     <sheet name="Via Adm" sheetId="2" r:id="rId2"/>
     <sheet name="Quantitativo Embalagens" sheetId="3" r:id="rId3"/>
     <sheet name="Quantitativo Embalagens Módulos" sheetId="4" r:id="rId4"/>
+    <sheet name="Hospitais para Cálculo" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Produto!$A$1:$B$249</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="319">
   <si>
     <t>Produto Prescrição</t>
   </si>
@@ -985,6 +986,9 @@
   </si>
   <si>
     <t>APTAMIL SOJA</t>
+  </si>
+  <si>
+    <t>Número Hospital</t>
   </si>
 </sst>
 </file>
@@ -1408,13 +1412,13 @@
       <selection pane="bottomLeft" activeCell="A248" sqref="A248"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.36328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1422,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>89</v>
       </c>
@@ -1430,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>90</v>
       </c>
@@ -1438,7 +1442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>91</v>
       </c>
@@ -1446,7 +1450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>92</v>
       </c>
@@ -1454,7 +1458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>93</v>
       </c>
@@ -1462,7 +1466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>94</v>
       </c>
@@ -1470,7 +1474,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>95</v>
       </c>
@@ -1478,7 +1482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>96</v>
       </c>
@@ -1486,7 +1490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>97</v>
       </c>
@@ -1494,7 +1498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>98</v>
       </c>
@@ -1502,7 +1506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>99</v>
       </c>
@@ -1510,7 +1514,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>100</v>
       </c>
@@ -1518,7 +1522,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>101</v>
       </c>
@@ -1526,7 +1530,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>102</v>
       </c>
@@ -1534,7 +1538,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>103</v>
       </c>
@@ -1542,7 +1546,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>104</v>
       </c>
@@ -1550,7 +1554,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>105</v>
       </c>
@@ -1558,7 +1562,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>106</v>
       </c>
@@ -1566,7 +1570,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>107</v>
       </c>
@@ -1574,7 +1578,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>108</v>
       </c>
@@ -1582,7 +1586,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>109</v>
       </c>
@@ -1590,7 +1594,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>110</v>
       </c>
@@ -1598,7 +1602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>111</v>
       </c>
@@ -1606,7 +1610,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>112</v>
       </c>
@@ -1614,7 +1618,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>113</v>
       </c>
@@ -1622,7 +1626,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>114</v>
       </c>
@@ -1630,7 +1634,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>25</v>
       </c>
@@ -1638,7 +1642,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>115</v>
       </c>
@@ -1646,7 +1650,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>116</v>
       </c>
@@ -1654,7 +1658,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>117</v>
       </c>
@@ -1662,7 +1666,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>118</v>
       </c>
@@ -1670,7 +1674,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>119</v>
       </c>
@@ -1678,7 +1682,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>120</v>
       </c>
@@ -1686,7 +1690,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>121</v>
       </c>
@@ -1694,7 +1698,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>122</v>
       </c>
@@ -1702,7 +1706,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>123</v>
       </c>
@@ -1710,7 +1714,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>124</v>
       </c>
@@ -1718,7 +1722,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>125</v>
       </c>
@@ -1726,7 +1730,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>126</v>
       </c>
@@ -1734,7 +1738,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>127</v>
       </c>
@@ -1742,7 +1746,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>128</v>
       </c>
@@ -1750,7 +1754,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>129</v>
       </c>
@@ -1758,7 +1762,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>130</v>
       </c>
@@ -1766,7 +1770,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>131</v>
       </c>
@@ -1774,7 +1778,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>132</v>
       </c>
@@ -1782,7 +1786,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>133</v>
       </c>
@@ -1790,7 +1794,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>134</v>
       </c>
@@ -1798,7 +1802,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>135</v>
       </c>
@@ -1806,7 +1810,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>136</v>
       </c>
@@ -1814,7 +1818,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>137</v>
       </c>
@@ -1822,7 +1826,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>26</v>
       </c>
@@ -1830,7 +1834,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>138</v>
       </c>
@@ -1838,7 +1842,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>139</v>
       </c>
@@ -1846,7 +1850,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>140</v>
       </c>
@@ -1854,7 +1858,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>141</v>
       </c>
@@ -1862,7 +1866,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>142</v>
       </c>
@@ -1870,7 +1874,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>143</v>
       </c>
@@ -1878,7 +1882,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>144</v>
       </c>
@@ -1886,7 +1890,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>145</v>
       </c>
@@ -1894,7 +1898,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>146</v>
       </c>
@@ -1902,7 +1906,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>147</v>
       </c>
@@ -1910,7 +1914,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>148</v>
       </c>
@@ -1918,7 +1922,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>149</v>
       </c>
@@ -1926,7 +1930,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>150</v>
       </c>
@@ -1934,7 +1938,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>151</v>
       </c>
@@ -1942,7 +1946,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>152</v>
       </c>
@@ -1950,7 +1954,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>153</v>
       </c>
@@ -1958,7 +1962,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>154</v>
       </c>
@@ -1966,7 +1970,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>155</v>
       </c>
@@ -1974,7 +1978,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>156</v>
       </c>
@@ -1982,7 +1986,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>157</v>
       </c>
@@ -1990,7 +1994,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>158</v>
       </c>
@@ -1998,7 +2002,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>27</v>
       </c>
@@ -2006,7 +2010,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>159</v>
       </c>
@@ -2014,7 +2018,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>160</v>
       </c>
@@ -2022,7 +2026,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>161</v>
       </c>
@@ -2030,7 +2034,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>162</v>
       </c>
@@ -2038,7 +2042,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>163</v>
       </c>
@@ -2046,7 +2050,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>164</v>
       </c>
@@ -2054,7 +2058,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>165</v>
       </c>
@@ -2062,7 +2066,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>166</v>
       </c>
@@ -2070,7 +2074,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>167</v>
       </c>
@@ -2078,7 +2082,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>168</v>
       </c>
@@ -2086,7 +2090,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>169</v>
       </c>
@@ -2094,7 +2098,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>170</v>
       </c>
@@ -2102,7 +2106,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>171</v>
       </c>
@@ -2110,7 +2114,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>172</v>
       </c>
@@ -2118,7 +2122,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>173</v>
       </c>
@@ -2126,7 +2130,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>174</v>
       </c>
@@ -2134,7 +2138,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>175</v>
       </c>
@@ -2142,7 +2146,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>176</v>
       </c>
@@ -2150,7 +2154,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>177</v>
       </c>
@@ -2158,7 +2162,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>178</v>
       </c>
@@ -2166,7 +2170,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>179</v>
       </c>
@@ -2174,7 +2178,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>180</v>
       </c>
@@ -2182,7 +2186,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>181</v>
       </c>
@@ -2190,7 +2194,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>182</v>
       </c>
@@ -2198,7 +2202,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>28</v>
       </c>
@@ -2206,7 +2210,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>183</v>
       </c>
@@ -2214,7 +2218,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>184</v>
       </c>
@@ -2222,7 +2226,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>29</v>
       </c>
@@ -2230,7 +2234,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>185</v>
       </c>
@@ -2238,7 +2242,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>30</v>
       </c>
@@ -2246,7 +2250,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>31</v>
       </c>
@@ -2254,7 +2258,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>186</v>
       </c>
@@ -2262,7 +2266,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>187</v>
       </c>
@@ -2270,7 +2274,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>32</v>
       </c>
@@ -2278,7 +2282,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>33</v>
       </c>
@@ -2286,7 +2290,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>315</v>
       </c>
@@ -2294,7 +2298,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>34</v>
       </c>
@@ -2302,7 +2306,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>188</v>
       </c>
@@ -2310,7 +2314,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>189</v>
       </c>
@@ -2318,7 +2322,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>190</v>
       </c>
@@ -2326,7 +2330,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>191</v>
       </c>
@@ -2334,7 +2338,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>192</v>
       </c>
@@ -2342,7 +2346,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>193</v>
       </c>
@@ -2350,7 +2354,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>316</v>
       </c>
@@ -2358,7 +2362,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>194</v>
       </c>
@@ -2366,7 +2370,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
         <v>195</v>
       </c>
@@ -2374,7 +2378,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
         <v>196</v>
       </c>
@@ -2382,7 +2386,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>197</v>
       </c>
@@ -2390,7 +2394,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>198</v>
       </c>
@@ -2398,7 +2402,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>35</v>
       </c>
@@ -2406,7 +2410,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
         <v>199</v>
       </c>
@@ -2414,7 +2418,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>200</v>
       </c>
@@ -2422,7 +2426,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>36</v>
       </c>
@@ -2430,7 +2434,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>201</v>
       </c>
@@ -2438,7 +2442,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
         <v>202</v>
       </c>
@@ -2446,7 +2450,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
         <v>203</v>
       </c>
@@ -2454,7 +2458,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
         <v>204</v>
       </c>
@@ -2462,7 +2466,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>205</v>
       </c>
@@ -2470,7 +2474,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
         <v>206</v>
       </c>
@@ -2478,7 +2482,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>207</v>
       </c>
@@ -2486,7 +2490,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>208</v>
       </c>
@@ -2494,7 +2498,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
         <v>209</v>
       </c>
@@ -2502,7 +2506,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>210</v>
       </c>
@@ -2510,7 +2514,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>37</v>
       </c>
@@ -2518,7 +2522,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>38</v>
       </c>
@@ -2526,7 +2530,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
         <v>211</v>
       </c>
@@ -2534,7 +2538,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
         <v>212</v>
       </c>
@@ -2542,7 +2546,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
         <v>213</v>
       </c>
@@ -2550,7 +2554,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
         <v>214</v>
       </c>
@@ -2558,7 +2562,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
         <v>215</v>
       </c>
@@ -2566,7 +2570,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
         <v>39</v>
       </c>
@@ -2574,7 +2578,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
         <v>216</v>
       </c>
@@ -2582,7 +2586,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
         <v>217</v>
       </c>
@@ -2590,7 +2594,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
         <v>218</v>
       </c>
@@ -2598,7 +2602,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>219</v>
       </c>
@@ -2606,7 +2610,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>220</v>
       </c>
@@ -2614,7 +2618,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>221</v>
       </c>
@@ -2622,7 +2626,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>222</v>
       </c>
@@ -2630,7 +2634,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
         <v>40</v>
       </c>
@@ -2638,7 +2642,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
         <v>223</v>
       </c>
@@ -2646,7 +2650,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>224</v>
       </c>
@@ -2654,7 +2658,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>225</v>
       </c>
@@ -2662,7 +2666,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>226</v>
       </c>
@@ -2670,7 +2674,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>227</v>
       </c>
@@ -2678,7 +2682,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
         <v>228</v>
       </c>
@@ -2686,7 +2690,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
         <v>229</v>
       </c>
@@ -2694,7 +2698,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
         <v>230</v>
       </c>
@@ -2702,7 +2706,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
         <v>231</v>
       </c>
@@ -2710,7 +2714,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
         <v>232</v>
       </c>
@@ -2718,7 +2722,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
         <v>233</v>
       </c>
@@ -2726,7 +2730,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
         <v>234</v>
       </c>
@@ -2734,7 +2738,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
         <v>235</v>
       </c>
@@ -2742,7 +2746,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
         <v>236</v>
       </c>
@@ -2750,7 +2754,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
         <v>237</v>
       </c>
@@ -2758,7 +2762,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
         <v>238</v>
       </c>
@@ -2766,7 +2770,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
         <v>239</v>
       </c>
@@ -2774,7 +2778,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
         <v>240</v>
       </c>
@@ -2782,7 +2786,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
         <v>241</v>
       </c>
@@ -2790,7 +2794,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
         <v>242</v>
       </c>
@@ -2798,7 +2802,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="7" t="s">
         <v>243</v>
       </c>
@@ -2806,7 +2810,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="7" t="s">
         <v>244</v>
       </c>
@@ -2814,7 +2818,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="7" t="s">
         <v>245</v>
       </c>
@@ -2822,7 +2826,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
         <v>246</v>
       </c>
@@ -2830,7 +2834,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="7" t="s">
         <v>247</v>
       </c>
@@ -2838,7 +2842,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
         <v>247</v>
       </c>
@@ -2846,7 +2850,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="7" t="s">
         <v>247</v>
       </c>
@@ -2854,7 +2858,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
         <v>248</v>
       </c>
@@ -2862,7 +2866,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="7" t="s">
         <v>249</v>
       </c>
@@ -2870,7 +2874,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
         <v>249</v>
       </c>
@@ -2878,7 +2882,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
         <v>250</v>
       </c>
@@ -2886,7 +2890,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="7" t="s">
         <v>251</v>
       </c>
@@ -2894,7 +2898,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="7" t="s">
         <v>252</v>
       </c>
@@ -2902,7 +2906,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="7" t="s">
         <v>253</v>
       </c>
@@ -2910,7 +2914,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="7" t="s">
         <v>254</v>
       </c>
@@ -2918,7 +2922,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
         <v>255</v>
       </c>
@@ -2926,7 +2930,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
         <v>256</v>
       </c>
@@ -2934,7 +2938,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="7" t="s">
         <v>257</v>
       </c>
@@ -2942,7 +2946,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="7" t="s">
         <v>258</v>
       </c>
@@ -2950,7 +2954,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="7" t="s">
         <v>259</v>
       </c>
@@ -2958,7 +2962,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="7" t="s">
         <v>41</v>
       </c>
@@ -2966,7 +2970,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="7" t="s">
         <v>260</v>
       </c>
@@ -2974,7 +2978,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="7" t="s">
         <v>261</v>
       </c>
@@ -2982,7 +2986,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
         <v>262</v>
       </c>
@@ -2990,7 +2994,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
         <v>263</v>
       </c>
@@ -2998,7 +3002,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="7" t="s">
         <v>264</v>
       </c>
@@ -3006,7 +3010,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="7" t="s">
         <v>265</v>
       </c>
@@ -3014,7 +3018,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="7" t="s">
         <v>266</v>
       </c>
@@ -3022,7 +3026,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="7" t="s">
         <v>267</v>
       </c>
@@ -3030,7 +3034,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="7" t="s">
         <v>42</v>
       </c>
@@ -3038,7 +3042,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="7" t="s">
         <v>268</v>
       </c>
@@ -3046,7 +3050,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="7" t="s">
         <v>269</v>
       </c>
@@ -3054,7 +3058,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="7" t="s">
         <v>43</v>
       </c>
@@ -3062,7 +3066,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="7" t="s">
         <v>312</v>
       </c>
@@ -3070,7 +3074,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="7" t="s">
         <v>313</v>
       </c>
@@ -3078,7 +3082,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="7" t="s">
         <v>270</v>
       </c>
@@ -3086,7 +3090,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="7" t="s">
         <v>314</v>
       </c>
@@ -3094,7 +3098,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="7" t="s">
         <v>271</v>
       </c>
@@ -3102,7 +3106,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
         <v>272</v>
       </c>
@@ -3110,7 +3114,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="7" t="s">
         <v>273</v>
       </c>
@@ -3118,7 +3122,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="7" t="s">
         <v>274</v>
       </c>
@@ -3126,7 +3130,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="7" t="s">
         <v>275</v>
       </c>
@@ -3134,7 +3138,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="7" t="s">
         <v>276</v>
       </c>
@@ -3142,7 +3146,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="7" t="s">
         <v>277</v>
       </c>
@@ -3150,7 +3154,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="7" t="s">
         <v>278</v>
       </c>
@@ -3158,7 +3162,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="7" t="s">
         <v>279</v>
       </c>
@@ -3166,7 +3170,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="7" t="s">
         <v>280</v>
       </c>
@@ -3174,7 +3178,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="7" t="s">
         <v>281</v>
       </c>
@@ -3182,7 +3186,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="7" t="s">
         <v>282</v>
       </c>
@@ -3190,7 +3194,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="7" t="s">
         <v>283</v>
       </c>
@@ -3198,7 +3202,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="7" t="s">
         <v>44</v>
       </c>
@@ -3206,7 +3210,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="7" t="s">
         <v>309</v>
       </c>
@@ -3214,7 +3218,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="7" t="s">
         <v>310</v>
       </c>
@@ -3222,7 +3226,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="7" t="s">
         <v>311</v>
       </c>
@@ -3230,7 +3234,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="7" t="s">
         <v>284</v>
       </c>
@@ -3238,7 +3242,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="7" t="s">
         <v>285</v>
       </c>
@@ -3246,7 +3250,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="7" t="s">
         <v>286</v>
       </c>
@@ -3254,7 +3258,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="7" t="s">
         <v>287</v>
       </c>
@@ -3262,7 +3266,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="7" t="s">
         <v>288</v>
       </c>
@@ -3270,7 +3274,7 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="7" t="s">
         <v>289</v>
       </c>
@@ -3278,7 +3282,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="7" t="s">
         <v>290</v>
       </c>
@@ -3286,7 +3290,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="7" t="s">
         <v>291</v>
       </c>
@@ -3294,7 +3298,7 @@
         <v>1122</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="7" t="s">
         <v>292</v>
       </c>
@@ -3302,7 +3306,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="7" t="s">
         <v>293</v>
       </c>
@@ -3310,7 +3314,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="7" t="s">
         <v>294</v>
       </c>
@@ -3318,7 +3322,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="7" t="s">
         <v>295</v>
       </c>
@@ -3326,7 +3330,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="7" t="s">
         <v>296</v>
       </c>
@@ -3334,7 +3338,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="7" t="s">
         <v>297</v>
       </c>
@@ -3342,7 +3346,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="7" t="s">
         <v>298</v>
       </c>
@@ -3350,7 +3354,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="7" t="s">
         <v>299</v>
       </c>
@@ -3358,7 +3362,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="7" t="s">
         <v>300</v>
       </c>
@@ -3366,7 +3370,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="7" t="s">
         <v>301</v>
       </c>
@@ -3374,7 +3378,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="7" t="s">
         <v>302</v>
       </c>
@@ -3382,7 +3386,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="7" t="s">
         <v>317</v>
       </c>
@@ -3390,7 +3394,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="7" t="s">
         <v>304</v>
       </c>
@@ -3398,7 +3402,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="7" t="s">
         <v>305</v>
       </c>
@@ -3424,13 +3428,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.90625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3438,7 +3442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>303</v>
       </c>
@@ -3446,7 +3450,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
@@ -3454,7 +3458,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -3462,7 +3466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3470,7 +3474,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3478,7 +3482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -3487,7 +3491,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B7">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B7">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3504,16 +3508,16 @@
       <selection pane="bottomLeft" activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
@@ -3530,7 +3534,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>4</v>
       </c>
@@ -3547,7 +3551,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>4</v>
       </c>
@@ -3564,7 +3568,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>4</v>
       </c>
@@ -3581,7 +3585,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -3598,7 +3602,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -3615,7 +3619,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>4</v>
       </c>
@@ -3632,7 +3636,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>4</v>
       </c>
@@ -3649,7 +3653,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>4</v>
       </c>
@@ -3666,7 +3670,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>4</v>
       </c>
@@ -3683,7 +3687,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>4</v>
       </c>
@@ -3700,7 +3704,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>4</v>
       </c>
@@ -3717,7 +3721,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>4</v>
       </c>
@@ -3734,7 +3738,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>4</v>
       </c>
@@ -3751,7 +3755,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>4</v>
       </c>
@@ -3768,7 +3772,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>4</v>
       </c>
@@ -3785,7 +3789,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>4</v>
       </c>
@@ -3802,7 +3806,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>4</v>
       </c>
@@ -3819,7 +3823,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>4</v>
       </c>
@@ -3836,7 +3840,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>4</v>
       </c>
@@ -3853,7 +3857,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>4</v>
       </c>
@@ -3870,7 +3874,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>25</v>
       </c>
@@ -3887,7 +3891,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>25</v>
       </c>
@@ -3904,7 +3908,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>25</v>
       </c>
@@ -3921,7 +3925,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>25</v>
       </c>
@@ -3938,7 +3942,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -3955,7 +3959,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -3972,7 +3976,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>25</v>
       </c>
@@ -3989,7 +3993,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>25</v>
       </c>
@@ -4006,7 +4010,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>25</v>
       </c>
@@ -4023,7 +4027,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>25</v>
       </c>
@@ -4040,7 +4044,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>25</v>
       </c>
@@ -4057,7 +4061,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>25</v>
       </c>
@@ -4074,7 +4078,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>25</v>
       </c>
@@ -4091,7 +4095,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>25</v>
       </c>
@@ -4108,7 +4112,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>25</v>
       </c>
@@ -4125,7 +4129,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>25</v>
       </c>
@@ -4142,7 +4146,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>25</v>
       </c>
@@ -4159,7 +4163,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>25</v>
       </c>
@@ -4176,7 +4180,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>25</v>
       </c>
@@ -4193,7 +4197,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>25</v>
       </c>
@@ -4210,7 +4214,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>25</v>
       </c>
@@ -4227,7 +4231,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>25</v>
       </c>
@@ -4244,7 +4248,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>28</v>
       </c>
@@ -4261,7 +4265,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>28</v>
       </c>
@@ -4278,7 +4282,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>28</v>
       </c>
@@ -4295,7 +4299,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>28</v>
       </c>
@@ -4312,7 +4316,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>28</v>
       </c>
@@ -4329,7 +4333,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>28</v>
       </c>
@@ -4346,7 +4350,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>28</v>
       </c>
@@ -4363,7 +4367,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>28</v>
       </c>
@@ -4380,7 +4384,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>28</v>
       </c>
@@ -4397,7 +4401,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>28</v>
       </c>
@@ -4414,7 +4418,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>28</v>
       </c>
@@ -4431,7 +4435,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>28</v>
       </c>
@@ -4448,7 +4452,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>28</v>
       </c>
@@ -4465,7 +4469,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>28</v>
       </c>
@@ -4482,7 +4486,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>28</v>
       </c>
@@ -4499,7 +4503,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>28</v>
       </c>
@@ -4516,7 +4520,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>28</v>
       </c>
@@ -4533,7 +4537,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>28</v>
       </c>
@@ -4550,7 +4554,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>28</v>
       </c>
@@ -4567,7 +4571,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>28</v>
       </c>
@@ -4584,7 +4588,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>28</v>
       </c>
@@ -4601,7 +4605,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>28</v>
       </c>
@@ -4618,7 +4622,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <v>28</v>
       </c>
@@ -4635,7 +4639,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>28</v>
       </c>
@@ -4652,7 +4656,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>49</v>
       </c>
@@ -4669,7 +4673,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>49</v>
       </c>
@@ -4686,7 +4690,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>49</v>
       </c>
@@ -4703,7 +4707,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>49</v>
       </c>
@@ -4720,7 +4724,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>49</v>
       </c>
@@ -4737,7 +4741,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>49</v>
       </c>
@@ -4754,7 +4758,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>49</v>
       </c>
@@ -4771,7 +4775,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>49</v>
       </c>
@@ -4788,7 +4792,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>49</v>
       </c>
@@ -4805,7 +4809,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>49</v>
       </c>
@@ -4822,7 +4826,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>49</v>
       </c>
@@ -4839,7 +4843,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>49</v>
       </c>
@@ -4856,7 +4860,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>49</v>
       </c>
@@ -4873,7 +4877,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>49</v>
       </c>
@@ -4890,7 +4894,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>49</v>
       </c>
@@ -4907,7 +4911,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>49</v>
       </c>
@@ -4924,7 +4928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>49</v>
       </c>
@@ -4941,7 +4945,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>49</v>
       </c>
@@ -4958,7 +4962,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>49</v>
       </c>
@@ -4975,7 +4979,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>49</v>
       </c>
@@ -4992,7 +4996,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>49</v>
       </c>
@@ -5009,7 +5013,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>49</v>
       </c>
@@ -5026,7 +5030,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>49</v>
       </c>
@@ -5043,7 +5047,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>49</v>
       </c>
@@ -5060,7 +5064,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="8">
         <v>17</v>
       </c>
@@ -5077,7 +5081,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="8">
         <v>17</v>
       </c>
@@ -5094,7 +5098,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="8">
         <v>17</v>
       </c>
@@ -5111,7 +5115,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <v>17</v>
       </c>
@@ -5128,7 +5132,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="8">
         <v>17</v>
       </c>
@@ -5145,7 +5149,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="8">
         <v>17</v>
       </c>
@@ -5162,7 +5166,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="8">
         <v>17</v>
       </c>
@@ -5179,7 +5183,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
         <v>17</v>
       </c>
@@ -5196,7 +5200,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="8">
         <v>17</v>
       </c>
@@ -5213,7 +5217,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="8">
         <v>17</v>
       </c>
@@ -5230,7 +5234,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="8">
         <v>17</v>
       </c>
@@ -5247,7 +5251,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
         <v>17</v>
       </c>
@@ -5264,7 +5268,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="8">
         <v>17</v>
       </c>
@@ -5281,7 +5285,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="8">
         <v>17</v>
       </c>
@@ -5298,7 +5302,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="8">
         <v>17</v>
       </c>
@@ -5315,7 +5319,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="8">
         <v>17</v>
       </c>
@@ -5332,7 +5336,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="8">
         <v>17</v>
       </c>
@@ -5349,7 +5353,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="8">
         <v>17</v>
       </c>
@@ -5366,7 +5370,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="8">
         <v>17</v>
       </c>
@@ -5383,7 +5387,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="8">
         <v>17</v>
       </c>
@@ -5400,7 +5404,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="8">
         <v>17</v>
       </c>
@@ -5417,7 +5421,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="8">
         <v>17</v>
       </c>
@@ -5444,21 +5448,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6511EA6E-EB8B-4E1E-AAE4-D6B9ED491513}">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
@@ -5475,7 +5479,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>4</v>
       </c>
@@ -5492,7 +5496,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>4</v>
       </c>
@@ -5509,7 +5513,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>4</v>
       </c>
@@ -5526,7 +5530,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -5543,7 +5547,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -5560,7 +5564,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>4</v>
       </c>
@@ -5577,7 +5581,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>4</v>
       </c>
@@ -5594,7 +5598,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>4</v>
       </c>
@@ -5611,7 +5615,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>4</v>
       </c>
@@ -5628,7 +5632,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>4</v>
       </c>
@@ -5645,7 +5649,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>4</v>
       </c>
@@ -5662,7 +5666,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>4</v>
       </c>
@@ -5679,7 +5683,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>4</v>
       </c>
@@ -5696,7 +5700,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>4</v>
       </c>
@@ -5713,7 +5717,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>4</v>
       </c>
@@ -5730,7 +5734,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>4</v>
       </c>
@@ -5747,7 +5751,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>4</v>
       </c>
@@ -5764,7 +5768,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>4</v>
       </c>
@@ -5781,7 +5785,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>4</v>
       </c>
@@ -5798,7 +5802,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>25</v>
       </c>
@@ -5815,7 +5819,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>25</v>
       </c>
@@ -5832,7 +5836,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>25</v>
       </c>
@@ -5849,7 +5853,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>25</v>
       </c>
@@ -5866,7 +5870,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>25</v>
       </c>
@@ -5883,7 +5887,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -5900,7 +5904,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -5917,7 +5921,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>25</v>
       </c>
@@ -5934,7 +5938,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>25</v>
       </c>
@@ -5951,7 +5955,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>25</v>
       </c>
@@ -5968,7 +5972,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>25</v>
       </c>
@@ -5985,7 +5989,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>25</v>
       </c>
@@ -6002,7 +6006,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>25</v>
       </c>
@@ -6019,7 +6023,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>25</v>
       </c>
@@ -6036,7 +6040,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>25</v>
       </c>
@@ -6053,7 +6057,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>25</v>
       </c>
@@ -6070,7 +6074,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>25</v>
       </c>
@@ -6087,7 +6091,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>25</v>
       </c>
@@ -6104,7 +6108,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>25</v>
       </c>
@@ -6121,7 +6125,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>25</v>
       </c>
@@ -6138,7 +6142,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>28</v>
       </c>
@@ -6155,7 +6159,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>28</v>
       </c>
@@ -6172,7 +6176,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>28</v>
       </c>
@@ -6189,7 +6193,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>28</v>
       </c>
@@ -6206,7 +6210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>28</v>
       </c>
@@ -6223,7 +6227,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>28</v>
       </c>
@@ -6240,7 +6244,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>28</v>
       </c>
@@ -6257,7 +6261,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>28</v>
       </c>
@@ -6274,7 +6278,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>28</v>
       </c>
@@ -6291,7 +6295,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>28</v>
       </c>
@@ -6308,7 +6312,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>28</v>
       </c>
@@ -6325,7 +6329,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>28</v>
       </c>
@@ -6342,7 +6346,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>28</v>
       </c>
@@ -6359,7 +6363,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>28</v>
       </c>
@@ -6376,7 +6380,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>28</v>
       </c>
@@ -6393,7 +6397,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>28</v>
       </c>
@@ -6410,7 +6414,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>28</v>
       </c>
@@ -6427,7 +6431,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>28</v>
       </c>
@@ -6444,7 +6448,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>28</v>
       </c>
@@ -6461,7 +6465,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>28</v>
       </c>
@@ -6478,7 +6482,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>28</v>
       </c>
@@ -6495,7 +6499,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>28</v>
       </c>
@@ -6512,7 +6516,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>28</v>
       </c>
@@ -6529,7 +6533,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>28</v>
       </c>
@@ -6546,7 +6550,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>49</v>
       </c>
@@ -6563,7 +6567,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>49</v>
       </c>
@@ -6580,7 +6584,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>49</v>
       </c>
@@ -6597,7 +6601,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>49</v>
       </c>
@@ -6614,7 +6618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>49</v>
       </c>
@@ -6631,7 +6635,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>49</v>
       </c>
@@ -6648,7 +6652,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>49</v>
       </c>
@@ -6665,7 +6669,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>49</v>
       </c>
@@ -6682,7 +6686,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>49</v>
       </c>
@@ -6699,7 +6703,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>49</v>
       </c>
@@ -6716,7 +6720,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>49</v>
       </c>
@@ -6733,7 +6737,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>49</v>
       </c>
@@ -6750,7 +6754,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>49</v>
       </c>
@@ -6767,7 +6771,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>49</v>
       </c>
@@ -6784,7 +6788,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>49</v>
       </c>
@@ -6801,7 +6805,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>49</v>
       </c>
@@ -6818,7 +6822,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>49</v>
       </c>
@@ -6835,7 +6839,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>49</v>
       </c>
@@ -6852,7 +6856,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>49</v>
       </c>
@@ -6869,7 +6873,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>49</v>
       </c>
@@ -6886,7 +6890,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>49</v>
       </c>
@@ -6903,7 +6907,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>49</v>
       </c>
@@ -6920,7 +6924,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>49</v>
       </c>
@@ -6941,4 +6945,37 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E62ECE2-371B-403F-BE7A-91D824C0D31B}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>